<commit_message>
Completed 'm' going to do some reading on Hands-on for now
</commit_message>
<xml_diff>
--- a/documentation/completion-log.xlsx
+++ b/documentation/completion-log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Progress</t>
   </si>
@@ -394,7 +394,7 @@
   <dimension ref="A4:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,6 +549,12 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2">
+        <v>43607</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="str">

</xml_diff>

<commit_message>
Completed q, pretty low number
</commit_message>
<xml_diff>
--- a/documentation/completion-log.xlsx
+++ b/documentation/completion-log.xlsx
@@ -32,9 +32,6 @@
     <t>Letter</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A4:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,15 +427,15 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <v>43600</v>
@@ -443,10 +443,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
         <v>43601</v>
@@ -454,10 +454,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1">
         <v>43606</v>
@@ -465,10 +465,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1">
         <v>43606</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1">
         <v>43600</v>
@@ -487,10 +487,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1">
         <v>43606</v>
@@ -498,10 +498,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1">
         <v>43606</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1">
         <v>43606</v>
@@ -520,10 +520,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1">
         <v>43606</v>
@@ -535,7 +535,7 @@
         <v>j</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1">
         <v>43607</v>
@@ -547,7 +547,7 @@
         <v>k</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
         <v>43608</v>
@@ -559,7 +559,7 @@
         <v>l</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1">
         <v>43607</v>
@@ -571,7 +571,7 @@
         <v>m</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1">
         <v>43607</v>
@@ -583,7 +583,7 @@
         <v>n</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1">
         <v>43607</v>
@@ -595,7 +595,7 @@
         <v>o</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1">
         <v>43608</v>
@@ -607,7 +607,7 @@
         <v>p</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1">
         <v>43608</v>
@@ -618,8 +618,11 @@
         <f t="shared" si="0"/>
         <v>q</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <v>43613</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -628,7 +631,7 @@
         <v>r</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -637,7 +640,7 @@
         <v>s</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -646,7 +649,7 @@
         <v>t</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -655,7 +658,7 @@
         <v>u</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -664,7 +667,7 @@
         <v>v</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -673,7 +676,7 @@
         <v>w</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -682,7 +685,7 @@
         <v>x</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -691,7 +694,7 @@
         <v>y</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -700,15 +703,15 @@
         <v>z</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -717,7 +720,7 @@
         <v>B</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -726,7 +729,7 @@
         <v>C</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -735,7 +738,7 @@
         <v>D</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -744,7 +747,7 @@
         <v>E</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -753,7 +756,7 @@
         <v>F</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -762,7 +765,7 @@
         <v>G</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -771,7 +774,7 @@
         <v>H</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -780,7 +783,7 @@
         <v>I</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -789,7 +792,7 @@
         <v>J</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -798,7 +801,7 @@
         <v>K</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
@@ -807,7 +810,7 @@
         <v>L</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -816,7 +819,7 @@
         <v>M</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -825,7 +828,7 @@
         <v>N</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -834,7 +837,7 @@
         <v>O</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -843,7 +846,7 @@
         <v>P</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
@@ -852,7 +855,7 @@
         <v>Q</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -861,7 +864,7 @@
         <v>R</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
@@ -870,7 +873,7 @@
         <v>S</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
@@ -879,7 +882,7 @@
         <v>T</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
@@ -888,7 +891,7 @@
         <v>U</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
@@ -897,7 +900,7 @@
         <v>V</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
@@ -906,7 +909,7 @@
         <v>W</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
@@ -915,7 +918,7 @@
         <v>X</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
@@ -924,7 +927,7 @@
         <v>Y</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
@@ -933,7 +936,7 @@
         <v>Z</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed all documentation of upper case letters, will need to supplement a few characters.
</commit_message>
<xml_diff>
--- a/documentation/completion-log.xlsx
+++ b/documentation/completion-log.xlsx
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,8 +906,8 @@
       <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>13</v>
+      <c r="C32" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -920,8 +920,8 @@
         <f xml:space="preserve"> CHAR(CODE(B32) +1)</f>
         <v>B</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>13</v>
+      <c r="C33" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -934,8 +934,8 @@
         <f t="shared" ref="B34:B57" si="1" xml:space="preserve"> CHAR(CODE(B33) +1)</f>
         <v>C</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>13</v>
+      <c r="C34" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -948,8 +948,8 @@
         <f t="shared" si="1"/>
         <v>D</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>13</v>
+      <c r="C35" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -962,8 +962,8 @@
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>13</v>
+      <c r="C36" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -976,8 +976,8 @@
         <f t="shared" si="1"/>
         <v>F</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>13</v>
+      <c r="C37" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -990,8 +990,8 @@
         <f t="shared" si="1"/>
         <v>G</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>13</v>
+      <c r="C38" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1004,10 +1004,12 @@
         <f t="shared" si="1"/>
         <v>H</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="2"/>
+      <c r="C39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="4">
+        <v>43627</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -1018,10 +1020,12 @@
         <f t="shared" si="1"/>
         <v>I</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="2"/>
+      <c r="C40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="4">
+        <v>43627</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1032,8 +1036,8 @@
         <f t="shared" si="1"/>
         <v>J</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>13</v>
+      <c r="C41" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1046,8 +1050,8 @@
         <f t="shared" si="1"/>
         <v>K</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>13</v>
+      <c r="C42" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1074,8 +1078,8 @@
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>13</v>
+      <c r="C44" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1088,8 +1092,8 @@
         <f t="shared" si="1"/>
         <v>N</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>13</v>
+      <c r="C45" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1116,8 +1120,8 @@
         <f t="shared" si="1"/>
         <v>P</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>13</v>
+      <c r="C47" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1130,8 +1134,8 @@
         <f t="shared" si="1"/>
         <v>Q</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>13</v>
+      <c r="C48" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1144,8 +1148,8 @@
         <f t="shared" si="1"/>
         <v>R</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>13</v>
+      <c r="C49" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1158,8 +1162,8 @@
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>13</v>
+      <c r="C50" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1172,8 +1176,8 @@
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>13</v>
+      <c r="C51" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1186,8 +1190,8 @@
         <f t="shared" si="1"/>
         <v>U</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>13</v>
+      <c r="C52" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1200,8 +1204,8 @@
         <f t="shared" si="1"/>
         <v>V</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>13</v>
+      <c r="C53" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1214,8 +1218,8 @@
         <f t="shared" si="1"/>
         <v>W</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>13</v>
+      <c r="C54" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1242,8 +1246,8 @@
         <f t="shared" si="1"/>
         <v>Y</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>13</v>
+      <c r="C56" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1256,8 +1260,8 @@
         <f t="shared" si="1"/>
         <v>Z</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>13</v>
+      <c r="C57" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>

</xml_diff>

<commit_message>
Completed test 2, starting overall test 3
</commit_message>
<xml_diff>
--- a/documentation/completion-log.xlsx
+++ b/documentation/completion-log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="23">
   <si>
     <t>Progress</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Completed</t>
@@ -123,7 +120,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,12 +130,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF2121"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,13 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1082,8 +1072,8 @@
         <f t="shared" si="1"/>
         <v>L</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>13</v>
+      <c r="C43" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1128,8 +1118,8 @@
         <f t="shared" si="1"/>
         <v>O</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>13</v>
+      <c r="C46" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1270,10 +1260,12 @@
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="2"/>
+      <c r="C55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="4">
+        <v>43635</v>
+      </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -1313,7 +1305,7 @@
     <row r="58" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>12</v>
@@ -1328,7 +1320,7 @@
     <row r="59" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>12</v>
@@ -1343,7 +1335,7 @@
     <row r="60" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>12</v>
@@ -1358,7 +1350,7 @@
     <row r="61" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>12</v>
@@ -1373,12 +1365,14 @@
     <row r="62" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="4">
+        <v>43635</v>
+      </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -1386,12 +1380,14 @@
     <row r="63" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="4">
+        <v>43635</v>
+      </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -1399,12 +1395,14 @@
     <row r="64" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="4">
+        <v>43635</v>
+      </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -1412,12 +1410,14 @@
     <row r="65" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="4">
+        <v>43635</v>
+      </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -1425,12 +1425,14 @@
     <row r="66" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="4">
+        <v>43635</v>
+      </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -1440,10 +1442,12 @@
       <c r="B67" s="2">
         <v>0</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="2"/>
+      <c r="C67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="4">
+        <v>43635</v>
+      </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -1454,10 +1458,12 @@
         <f xml:space="preserve"> B67+1</f>
         <v>1</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D68" s="2"/>
+      <c r="C68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="4">
+        <v>43635</v>
+      </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -1468,10 +1474,12 @@
         <f t="shared" ref="B69:B76" si="2" xml:space="preserve"> B68+1</f>
         <v>2</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="2"/>
+      <c r="C69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="4">
+        <v>43635</v>
+      </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -1482,10 +1490,12 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="2"/>
+      <c r="C70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="4">
+        <v>43635</v>
+      </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -1496,10 +1506,12 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="2"/>
+      <c r="C71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="4">
+        <v>43635</v>
+      </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -1510,10 +1522,12 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="2"/>
+      <c r="C72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="4">
+        <v>43635</v>
+      </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -1524,10 +1538,12 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="2"/>
+      <c r="C73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="4">
+        <v>43635</v>
+      </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -1538,10 +1554,12 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="2"/>
+      <c r="C74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="4">
+        <v>43635</v>
+      </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -1552,10 +1570,12 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C75" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="2"/>
+      <c r="C75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="4">
+        <v>43635</v>
+      </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -1566,10 +1586,12 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="2"/>
+      <c r="C76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="4">
+        <v>43635</v>
+      </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>

</xml_diff>